<commit_message>
add for parallel testing
</commit_message>
<xml_diff>
--- a/test-scenario/Sauce Demo - Test Case.xlsx
+++ b/test-scenario/Sauce Demo - Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProject\Java\MyProject\CucumberBDDProject\CucumberProject\test-scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B9679F-508F-43CA-9A45-57F2F07CC904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3DB69A-7A12-4196-9743-711ED4392AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{293820DC-2992-4C9C-B994-FC6B8BF047EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
   <si>
     <t>No</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Result</t>
   </si>
   <si>
     <t>Login Feature</t>
@@ -910,9 +907,6 @@
   </si>
   <si>
     <t>CHK-08</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <t>Positive</t>
@@ -1372,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089AA1EE-42FB-4881-8A47-006ECAE7E7B0}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,10 +1385,9 @@
     <col min="9" max="9" width="20" style="1" customWidth="1"/>
     <col min="10" max="10" width="25.42578125" style="1" customWidth="1"/>
     <col min="11" max="12" width="25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1431,362 +1424,332 @@
       <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="K2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="K3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="E6" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="L6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="J10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" s="7" t="s">
+      <c r="L10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3"/>
       <c r="E11" s="9"/>
       <c r="F11" s="3"/>
@@ -1796,9 +1759,8 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
       <c r="E12" s="9"/>
       <c r="F12" s="3"/>
@@ -1808,9 +1770,8 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="3"/>
       <c r="E13" s="9"/>
       <c r="F13" s="3"/>
@@ -1820,9 +1781,8 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
       <c r="E14" s="9"/>
       <c r="F14" s="3"/>
@@ -1832,9 +1792,8 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="3"/>
       <c r="E15" s="9"/>
       <c r="F15" s="3"/>
@@ -1844,9 +1803,8 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="3"/>
       <c r="E16" s="9"/>
       <c r="F16" s="3"/>
@@ -1856,9 +1814,8 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
       <c r="E17" s="9"/>
       <c r="F17" s="3"/>
@@ -1868,9 +1825,8 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
       <c r="E18" s="9"/>
       <c r="F18" s="3"/>
@@ -1880,9 +1836,8 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="3"/>
       <c r="E19" s="9"/>
       <c r="F19" s="3"/>
@@ -1892,9 +1847,8 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="3"/>
       <c r="E20" s="9"/>
       <c r="F20" s="3"/>
@@ -1904,9 +1858,8 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3"/>
       <c r="E21" s="9"/>
       <c r="F21" s="3"/>
@@ -1916,9 +1869,8 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="9"/>
-    </row>
-    <row r="22" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
       <c r="E22" s="9"/>
       <c r="F22" s="3"/>
@@ -1928,9 +1880,8 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="9"/>
-    </row>
-    <row r="23" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
       <c r="E23" s="9"/>
       <c r="F23" s="3"/>
@@ -1940,9 +1891,8 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="9"/>
-    </row>
-    <row r="24" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="9"/>
       <c r="F24" s="3"/>
@@ -1952,9 +1902,8 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="E25" s="9"/>
       <c r="F25" s="3"/>
@@ -1964,9 +1913,8 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="9"/>
-    </row>
-    <row r="26" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="E26" s="9"/>
       <c r="F26" s="3"/>
@@ -1976,9 +1924,8 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="9"/>
-    </row>
-    <row r="27" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
       <c r="E27" s="9"/>
       <c r="F27" s="3"/>
@@ -1988,9 +1935,8 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="9"/>
-    </row>
-    <row r="28" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="E28" s="9"/>
       <c r="F28" s="3"/>
@@ -2000,9 +1946,8 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="9"/>
-    </row>
-    <row r="29" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="E29" s="9"/>
       <c r="F29" s="3"/>
@@ -2012,9 +1957,8 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="9"/>
-    </row>
-    <row r="30" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
       <c r="E30" s="9"/>
       <c r="F30" s="3"/>
@@ -2024,9 +1968,8 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="9"/>
-    </row>
-    <row r="31" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="E31" s="9"/>
       <c r="F31" s="3"/>
@@ -2036,9 +1979,8 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="9"/>
-    </row>
-    <row r="32" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="3"/>
       <c r="E32" s="9"/>
       <c r="F32" s="3"/>
@@ -2048,9 +1990,8 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="9"/>
-    </row>
-    <row r="33" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="4:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D33" s="3"/>
       <c r="E33" s="9"/>
       <c r="F33" s="3"/>
@@ -2060,7 +2001,6 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>